<commit_message>
Updated Code for JBL Login Page
</commit_message>
<xml_diff>
--- a/src/main/resources/TestData.xlsx
+++ b/src/main/resources/TestData.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20228"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:801_{F41F049E-1647-4060-B9B0-278432849CA8}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:801_{26FF3E9B-D86E-472F-951D-2D40B377952E}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="19380" windowHeight="5895" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="15330" windowHeight="2145" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="ContactUs" sheetId="1" r:id="rId1"/>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="29">
   <si>
     <t>FirstName</t>
   </si>
@@ -177,7 +177,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -194,6 +194,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="2">
@@ -620,20 +621,20 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1F59755D-AF6A-445F-905F-F1A10C531AD2}">
-  <dimension ref="A1:C4"/>
+  <dimension ref="A1:D4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C5" sqref="C5"/>
+      <selection activeCell="C1" sqref="C1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="28.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" customWidth="true" width="22.140625" collapsed="true"/>
     <col min="2" max="2" customWidth="true" width="14.7109375" collapsed="true"/>
-    <col min="3" max="3" bestFit="true" customWidth="true" width="6.59375" collapsed="true"/>
+    <col min="4" max="4" bestFit="true" customWidth="true" width="6.59375" collapsed="true"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
         <v>22</v>
       </c>
@@ -643,37 +644,40 @@
       <c r="C1" t="s" s="6">
         <v>26</v>
       </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="D1" t="s" s="7">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>24</v>
       </c>
       <c r="B2" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="C2" t="s">
+      <c r="D2" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>24</v>
       </c>
       <c r="B3" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="C3" t="s">
+      <c r="D3" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
         <v>24</v>
       </c>
       <c r="B4" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="C4" t="s">
+      <c r="D4" t="s">
         <v>27</v>
       </c>
     </row>

</xml_diff>

<commit_message>
removed column for TestData Excel
</commit_message>
<xml_diff>
--- a/src/main/resources/TestData.xlsx
+++ b/src/main/resources/TestData.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20228"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:801_{26FF3E9B-D86E-472F-951D-2D40B377952E}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:801_{441E64A3-F318-4139-B7AD-2039D0EB5AAD}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="15330" windowHeight="2145" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -14,7 +14,7 @@
   <calcPr calcId="0"/>
   <oleSize ref="A1"/>
   <extLst>
-    <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
   </extLst>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="26">
   <si>
     <t>FirstName</t>
   </si>
@@ -100,22 +100,12 @@
   </si>
   <si>
     <t>changeme</t>
-  </si>
-  <si>
-    <t>Status</t>
-  </si>
-  <si>
-    <t>Fail</t>
-  </si>
-  <si>
-    <t>Pass</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="0"/>
   <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -177,7 +167,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -194,8 +184,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -485,12 +473,12 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" customWidth="true" width="15.140625" collapsed="true"/>
-    <col min="2" max="2" customWidth="true" width="14.7109375" collapsed="true"/>
-    <col min="3" max="3" customWidth="true" width="27.0" collapsed="true"/>
-    <col min="4" max="4" customWidth="true" width="18.42578125" collapsed="true"/>
-    <col min="5" max="5" bestFit="true" customWidth="true" width="37.0" collapsed="true"/>
-    <col min="6" max="6" customWidth="true" width="17.5703125" collapsed="true"/>
+    <col min="1" max="1" width="15.140625" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="14.7109375" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="27" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="18.42578125" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="37" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="6" max="6" width="17.5703125" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.25">
@@ -621,17 +609,16 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1F59755D-AF6A-445F-905F-F1A10C531AD2}">
-  <dimension ref="A1:D4"/>
+  <dimension ref="A1:G4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C1" sqref="C1"/>
+      <selection activeCell="C1" sqref="C1:D1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="28.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" customWidth="true" width="22.140625" collapsed="true"/>
-    <col min="2" max="2" customWidth="true" width="14.7109375" collapsed="true"/>
-    <col min="4" max="4" bestFit="true" customWidth="true" width="6.59375" collapsed="true"/>
+    <col min="1" max="1" width="22.140625" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="14.7109375" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.25">
@@ -641,12 +628,6 @@
       <c r="B1" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="C1" t="s" s="6">
-        <v>26</v>
-      </c>
-      <c r="D1" t="s" s="7">
-        <v>26</v>
-      </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
@@ -655,9 +636,6 @@
       <c r="B2" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="D2" t="s">
-        <v>27</v>
-      </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
@@ -666,9 +644,6 @@
       <c r="B3" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="D3" t="s">
-        <v>28</v>
-      </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
@@ -676,9 +651,6 @@
       </c>
       <c r="B4" s="1" t="s">
         <v>15</v>
-      </c>
-      <c r="D4" t="s">
-        <v>27</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added new Code for FreeCRM
</commit_message>
<xml_diff>
--- a/src/main/resources/TestData.xlsx
+++ b/src/main/resources/TestData.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20228"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:801_{683C3FB6-45B5-4372-9F75-7823D96E32E4}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:801_{D3A78C0F-87CA-4D7A-80AB-862CD131A0D9}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="11700" windowHeight="2145" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="15210" windowHeight="1980" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="ContactUs" sheetId="1" r:id="rId1"/>
@@ -612,7 +612,7 @@
   <dimension ref="A1:J4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C1" sqref="C1"/>
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="28.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>